<commit_message>
Prozessumbau: Manuelle Zuweisung bei keiner freien Position
</commit_message>
<xml_diff>
--- a/resourceplanning-client/src/main/resources/ManualTests.xlsx
+++ b/resourceplanning-client/src/main/resources/ManualTests.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2475" windowWidth="17565" windowHeight="5970"/>
+    <workbookView xWindow="0" yWindow="2475" windowWidth="19260" windowHeight="6705" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="1" r:id="rId1"/>
@@ -12,11 +12,12 @@
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="53">
   <si>
     <t>Aktion</t>
   </si>
@@ -166,6 +167,15 @@
   </si>
   <si>
     <t>Umlaute in Callback-JSP, ggf. in Auswahl-Mail ausweisen, dass es sich um eine wiederholte Abfrage handelt, da vorherige Wahl schon besetzt war?</t>
+  </si>
+  <si>
+    <t>Beim Vorschlagen von Positionen auf das Mindestalter eingehen</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Für verfügbare Positionen einen View bauen, der auch die zugehörige Domain enthält/anzeigt</t>
   </si>
 </sst>
 </file>
@@ -567,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -824,10 +834,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -835,14 +845,27 @@
     <col min="1" max="1" width="104.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>